<commit_message>
updated sampling ranges for experiment and added climate change factor to hydropower
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_ce_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_ce_calibrated.xlsx
@@ -609,10 +609,10 @@
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
         <v>0.3</v>
@@ -740,10 +740,10 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
         <v>0.195</v>
@@ -5063,10 +5063,10 @@
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J36" t="n">
         <v>0.31</v>
@@ -5456,10 +5456,10 @@
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I39" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J39" t="n">
         <v>0.6</v>
@@ -5587,10 +5587,10 @@
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I40" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J40" t="n">
         <v>0.25</v>
@@ -5718,10 +5718,10 @@
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>1.22</v>
+        <v>1</v>
       </c>
       <c r="I41" t="n">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="J41" t="n">
         <v>0.045</v>
@@ -5849,10 +5849,10 @@
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="I42" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
         <v>0.05</v>
@@ -5980,10 +5980,10 @@
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="I43" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J43" t="n">
         <v>0.025</v>
@@ -6111,10 +6111,10 @@
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>2.17</v>
+        <v>1</v>
       </c>
       <c r="I44" t="n">
-        <v>0.37</v>
+        <v>1</v>
       </c>
       <c r="J44" t="n">
         <v>1000</v>
@@ -6504,10 +6504,10 @@
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J47" t="n">
         <v>49</v>
@@ -6635,10 +6635,10 @@
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I48" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J48" t="n">
         <v>49</v>
@@ -6766,10 +6766,10 @@
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I49" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J49" t="n">
         <v>1000000</v>
@@ -6897,10 +6897,10 @@
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I50" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J50" t="n">
         <v>0.0014</v>
@@ -7028,10 +7028,10 @@
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I51" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J51" t="n">
         <v>0.0014</v>
@@ -7159,10 +7159,10 @@
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I52" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
         <v>0.0014</v>
@@ -7290,10 +7290,10 @@
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I53" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J53" t="n">
         <v>0.007</v>
@@ -7421,10 +7421,10 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I54" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J54" t="n">
         <v>0.007</v>
@@ -7552,10 +7552,10 @@
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I55" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J55" t="n">
         <v>0.007</v>
@@ -7683,10 +7683,10 @@
       <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I56" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J56" t="n">
         <v>0.0004199999999999</v>
@@ -7814,10 +7814,10 @@
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I57" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J57" t="n">
         <v>0.0004199999999999</v>
@@ -7945,10 +7945,10 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I58" t="n">
-        <v>0.57</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
         <v>0.0004199999999999</v>
@@ -8076,10 +8076,10 @@
       <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I59" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J59" t="n">
         <v>0.001</v>
@@ -8207,10 +8207,10 @@
       <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I60" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J60" t="n">
         <v>0.001</v>
@@ -8338,10 +8338,10 @@
       <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I61" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J61" t="n">
         <v>0.0001</v>
@@ -8469,10 +8469,10 @@
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I62" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J62" t="n">
         <v>8.670000000000001e-05</v>
@@ -8600,10 +8600,10 @@
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I63" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J63" t="n">
         <v>8.670000000000001e-05</v>
@@ -8731,10 +8731,10 @@
       <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I64" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J64" t="n">
         <v>8.670000000000001e-05</v>
@@ -8862,10 +8862,10 @@
       <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I65" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J65" t="n">
         <v>8.670000000000001e-05</v>
@@ -8993,10 +8993,10 @@
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I66" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J66" t="n">
         <v>8.670000000000001e-05</v>
@@ -9124,10 +9124,10 @@
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I67" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J67" t="n">
         <v>1e-05</v>
@@ -9255,10 +9255,10 @@
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I68" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J68" t="n">
         <v>0.00017</v>
@@ -9386,10 +9386,10 @@
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I69" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J69" t="n">
         <v>8.670000000000001e-05</v>
@@ -9517,10 +9517,10 @@
       <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="I70" t="n">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="J70" t="n">
         <v>0.000945</v>
@@ -9648,10 +9648,10 @@
       <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I71" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J71" t="n">
         <v>8.670000000000001e-05</v>
@@ -9779,10 +9779,10 @@
       <c r="F72" t="inlineStr"/>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I72" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J72" t="n">
         <v>1e-05</v>
@@ -9910,10 +9910,10 @@
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I73" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J73" t="n">
         <v>8.670000000000001e-05</v>
@@ -10172,10 +10172,10 @@
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
-        <v>16.66666666666667</v>
+        <v>1</v>
       </c>
       <c r="I75" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J75" t="n">
         <v>0.06</v>
@@ -10303,10 +10303,10 @@
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
-        <v>6.666666666666666</v>
+        <v>1</v>
       </c>
       <c r="I76" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J76" t="n">
         <v>0.15</v>
@@ -10434,10 +10434,10 @@
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="n">
-        <v>6.666666666666666</v>
+        <v>1</v>
       </c>
       <c r="I77" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J77" t="n">
         <v>0.15</v>
@@ -10565,10 +10565,10 @@
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="n">
-        <v>33.33333333333334</v>
+        <v>1</v>
       </c>
       <c r="I78" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J78" t="n">
         <v>0.03</v>
@@ -10696,10 +10696,10 @@
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="n">
-        <v>33.33333333333334</v>
+        <v>1</v>
       </c>
       <c r="I79" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J79" t="n">
         <v>0.03</v>
@@ -10827,10 +10827,10 @@
       <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="n">
-        <v>4.166666666666667</v>
+        <v>1</v>
       </c>
       <c r="I80" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J80" t="n">
         <v>0.24</v>
@@ -10958,10 +10958,10 @@
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
-        <v>6.666666666666666</v>
+        <v>1</v>
       </c>
       <c r="I81" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J81" t="n">
         <v>0.15</v>
@@ -11089,10 +11089,10 @@
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="n">
-        <v>6.666666666666666</v>
+        <v>1</v>
       </c>
       <c r="I82" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J82" t="n">
         <v>0.15</v>
@@ -11351,10 +11351,10 @@
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="n">
-        <v>33.33333333333334</v>
+        <v>1</v>
       </c>
       <c r="I84" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J84" t="n">
         <v>0.03</v>
@@ -11482,10 +11482,10 @@
       <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
-        <v>16.66666666666667</v>
+        <v>1</v>
       </c>
       <c r="I85" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J85" t="n">
         <v>0.06</v>
@@ -11613,10 +11613,10 @@
       <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="n">
-        <v>16.66666666666667</v>
+        <v>1</v>
       </c>
       <c r="I86" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J86" t="n">
         <v>0.06</v>
@@ -13971,10 +13971,10 @@
       <c r="F104" t="inlineStr"/>
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J104" t="n">
         <v>0.0162031455895955</v>
@@ -19604,10 +19604,10 @@
       <c r="F147" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
       <c r="H147" t="n">
-        <v>1.052631578947368</v>
+        <v>1</v>
       </c>
       <c r="I147" t="n">
-        <v>0.9473684210526316</v>
+        <v>1</v>
       </c>
       <c r="J147" t="n">
         <v>0.95</v>
@@ -19735,10 +19735,10 @@
       <c r="F148" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
       <c r="H148" t="n">
-        <v>1.052631578947368</v>
+        <v>1</v>
       </c>
       <c r="I148" t="n">
-        <v>0.9473684210526316</v>
+        <v>1</v>
       </c>
       <c r="J148" t="n">
         <v>0.95</v>
@@ -19866,10 +19866,10 @@
       <c r="F149" t="inlineStr"/>
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I149" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J149" t="n">
         <v>0.03</v>
@@ -19997,10 +19997,10 @@
       <c r="F150" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="n">
-        <v>1.66</v>
+        <v>1</v>
       </c>
       <c r="I150" t="n">
-        <v>0.76</v>
+        <v>1</v>
       </c>
       <c r="J150" t="n">
         <v>0.66</v>
@@ -20128,10 +20128,10 @@
       <c r="F151" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="n">
-        <v>1.66</v>
+        <v>1</v>
       </c>
       <c r="I151" t="n">
-        <v>0.76</v>
+        <v>1</v>
       </c>
       <c r="J151" t="n">
         <v>0.5</v>
@@ -20259,10 +20259,10 @@
       <c r="F152" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J152" t="n">
         <v>0.01</v>
@@ -20390,10 +20390,10 @@
       <c r="F153" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="n">
-        <v>1.17</v>
+        <v>1</v>
       </c>
       <c r="I153" t="n">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="J153" t="n">
         <v>0.094</v>
@@ -20521,10 +20521,10 @@
       <c r="F154" t="inlineStr"/>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="n">
-        <v>1.48</v>
+        <v>1</v>
       </c>
       <c r="I154" t="n">
-        <v>0.53</v>
+        <v>1</v>
       </c>
       <c r="J154" t="n">
         <v>0.183</v>
@@ -20914,10 +20914,10 @@
       <c r="F157" t="inlineStr"/>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="n">
-        <v>1.15</v>
+        <v>1</v>
       </c>
       <c r="I157" t="n">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="J157" t="n">
         <v>0.096</v>
@@ -21176,10 +21176,10 @@
       <c r="F159" t="inlineStr"/>
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="n">
-        <v>1.23</v>
+        <v>1</v>
       </c>
       <c r="I159" t="n">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="J159" t="n">
         <v>0.054</v>
@@ -21569,10 +21569,10 @@
       <c r="F162" t="inlineStr"/>
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="n">
-        <v>1.48</v>
+        <v>1</v>
       </c>
       <c r="I162" t="n">
-        <v>0.53</v>
+        <v>1</v>
       </c>
       <c r="J162" t="n">
         <v>0.183</v>
@@ -21700,10 +21700,10 @@
       <c r="F163" t="inlineStr"/>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="n">
-        <v>1.23</v>
+        <v>1</v>
       </c>
       <c r="I163" t="n">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="J163" t="n">
         <v>0.054</v>
@@ -21831,10 +21831,10 @@
       <c r="F164" t="inlineStr"/>
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="n">
-        <v>1.43</v>
+        <v>1</v>
       </c>
       <c r="I164" t="n">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="J164" t="n">
         <v>0.028</v>
@@ -21962,10 +21962,10 @@
       <c r="F165" t="inlineStr"/>
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="n">
-        <v>1.15</v>
+        <v>1</v>
       </c>
       <c r="I165" t="n">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="J165" t="n">
         <v>0.096</v>
@@ -22617,10 +22617,10 @@
       <c r="F170" t="inlineStr"/>
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="n">
-        <v>2.8125</v>
+        <v>1</v>
       </c>
       <c r="I170" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J170" t="n">
         <v>0.016</v>
@@ -22748,10 +22748,10 @@
       <c r="F171" t="inlineStr"/>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J171" t="n">
         <v>0.0005</v>
@@ -22879,10 +22879,10 @@
       <c r="F172" t="inlineStr"/>
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J172" t="n">
         <v>0.0005</v>
@@ -23010,10 +23010,10 @@
       <c r="F173" t="inlineStr"/>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J173" t="n">
         <v>0.0005</v>
@@ -23141,10 +23141,10 @@
       <c r="F174" t="inlineStr"/>
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="n">
-        <v>2.8125</v>
+        <v>1</v>
       </c>
       <c r="I174" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J174" t="n">
         <v>0.016</v>
@@ -23272,10 +23272,10 @@
       <c r="F175" t="inlineStr"/>
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="n">
-        <v>2.8125</v>
+        <v>1</v>
       </c>
       <c r="I175" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J175" t="n">
         <v>0.016</v>
@@ -23403,10 +23403,10 @@
       <c r="F176" t="inlineStr"/>
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J176" t="n">
         <v>0.0005</v>
@@ -23537,7 +23537,7 @@
         <v>1</v>
       </c>
       <c r="I177" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J177" t="n">
         <v>0.0025</v>
@@ -23665,10 +23665,10 @@
       <c r="F178" t="inlineStr"/>
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="n">
-        <v>7.58</v>
+        <v>1</v>
       </c>
       <c r="I178" t="n">
-        <v>0.042</v>
+        <v>1</v>
       </c>
       <c r="J178" t="n">
         <v>0.012</v>
@@ -23796,10 +23796,10 @@
       <c r="F179" t="inlineStr"/>
       <c r="G179" t="inlineStr"/>
       <c r="H179" t="n">
-        <v>7.58</v>
+        <v>1</v>
       </c>
       <c r="I179" t="n">
-        <v>0.042</v>
+        <v>1</v>
       </c>
       <c r="J179" t="n">
         <v>0.012</v>
@@ -23927,10 +23927,10 @@
       <c r="F180" t="inlineStr"/>
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="n">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="I180" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J180" t="n">
         <v>0.5</v>
@@ -24058,10 +24058,10 @@
       <c r="F181" t="inlineStr"/>
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="n">
-        <v>1.0625</v>
+        <v>1</v>
       </c>
       <c r="I181" t="n">
-        <v>0.5625</v>
+        <v>1</v>
       </c>
       <c r="J181" t="n">
         <v>0.8</v>
@@ -24189,10 +24189,10 @@
       <c r="F182" t="inlineStr"/>
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="n">
-        <v>1.0625</v>
+        <v>1</v>
       </c>
       <c r="I182" t="n">
-        <v>0.5625</v>
+        <v>1</v>
       </c>
       <c r="J182" t="n">
         <v>0.8</v>
@@ -24320,10 +24320,10 @@
       <c r="F183" t="inlineStr"/>
       <c r="G183" t="inlineStr"/>
       <c r="H183" t="n">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="I183" t="n">
-        <v>0.583</v>
+        <v>1</v>
       </c>
       <c r="J183" t="n">
         <v>0.12</v>
@@ -24451,10 +24451,10 @@
       <c r="F184" t="inlineStr"/>
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="n">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="I184" t="n">
-        <v>0.583</v>
+        <v>1</v>
       </c>
       <c r="J184" t="n">
         <v>0.12</v>
@@ -24582,10 +24582,10 @@
       <c r="F185" t="inlineStr"/>
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I185" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J185" t="n">
         <v>0.1</v>
@@ -24713,10 +24713,10 @@
       <c r="F186" t="inlineStr"/>
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="n">
-        <v>1.375</v>
+        <v>1</v>
       </c>
       <c r="I186" t="n">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="J186" t="n">
         <v>0.4</v>
@@ -24844,10 +24844,10 @@
       <c r="F187" t="inlineStr"/>
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="n">
-        <v>1.375</v>
+        <v>1</v>
       </c>
       <c r="I187" t="n">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="J187" t="n">
         <v>0.4</v>
@@ -24975,10 +24975,10 @@
       <c r="F188" t="inlineStr"/>
       <c r="G188" t="inlineStr"/>
       <c r="H188" t="n">
-        <v>1.67</v>
+        <v>1</v>
       </c>
       <c r="I188" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="J188" t="n">
         <v>0.15</v>
@@ -25368,10 +25368,10 @@
       <c r="F191" t="inlineStr"/>
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="n">
-        <v>1.333</v>
+        <v>1</v>
       </c>
       <c r="I191" t="n">
-        <v>0.833</v>
+        <v>1</v>
       </c>
       <c r="J191" t="n">
         <v>0.605</v>
@@ -25499,10 +25499,10 @@
       <c r="F192" t="inlineStr"/>
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="n">
-        <v>1.333</v>
+        <v>1</v>
       </c>
       <c r="I192" t="n">
-        <v>0.833</v>
+        <v>1</v>
       </c>
       <c r="J192" t="n">
         <v>0.605</v>
@@ -25633,7 +25633,7 @@
         <v>1</v>
       </c>
       <c r="I193" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J193" t="n">
         <v>0.098</v>
@@ -25764,7 +25764,7 @@
         <v>1</v>
       </c>
       <c r="I194" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J194" t="n">
         <v>0.098</v>
@@ -25895,7 +25895,7 @@
         <v>1</v>
       </c>
       <c r="I195" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J195" t="n">
         <v>0.35</v>
@@ -26026,7 +26026,7 @@
         <v>1</v>
       </c>
       <c r="I196" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J196" t="n">
         <v>0.35</v>
@@ -26157,7 +26157,7 @@
         <v>1</v>
       </c>
       <c r="I197" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J197" t="n">
         <v>0.35</v>
@@ -26288,7 +26288,7 @@
         <v>1</v>
       </c>
       <c r="I198" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J198" t="n">
         <v>0.098</v>
@@ -26678,10 +26678,10 @@
       <c r="F201" t="inlineStr"/>
       <c r="G201" t="inlineStr"/>
       <c r="H201" t="n">
-        <v>1.056</v>
+        <v>1</v>
       </c>
       <c r="I201" t="n">
-        <v>0.889</v>
+        <v>1</v>
       </c>
       <c r="J201" t="n">
         <v>0.9</v>
@@ -26809,10 +26809,10 @@
       <c r="F202" t="inlineStr"/>
       <c r="G202" t="inlineStr"/>
       <c r="H202" t="n">
-        <v>1.056</v>
+        <v>1</v>
       </c>
       <c r="I202" t="n">
-        <v>0.889</v>
+        <v>1</v>
       </c>
       <c r="J202" t="n">
         <v>0.9</v>
@@ -26940,10 +26940,10 @@
       <c r="F203" t="inlineStr"/>
       <c r="G203" t="inlineStr"/>
       <c r="H203" t="n">
-        <v>2.326</v>
+        <v>1</v>
       </c>
       <c r="I203" t="n">
-        <v>0.117</v>
+        <v>1</v>
       </c>
       <c r="J203" t="n">
         <v>0.6</v>
@@ -27071,10 +27071,10 @@
       <c r="F204" t="inlineStr"/>
       <c r="G204" t="inlineStr"/>
       <c r="H204" t="n">
-        <v>2.326</v>
+        <v>1</v>
       </c>
       <c r="I204" t="n">
-        <v>0.117</v>
+        <v>1</v>
       </c>
       <c r="J204" t="n">
         <v>0.1</v>
@@ -27202,10 +27202,10 @@
       <c r="F205" t="inlineStr"/>
       <c r="G205" t="inlineStr"/>
       <c r="H205" t="n">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="I205" t="n">
-        <v>0.625</v>
+        <v>1</v>
       </c>
       <c r="J205" t="n">
         <v>0.4</v>
@@ -27333,10 +27333,10 @@
       <c r="F206" t="inlineStr"/>
       <c r="G206" t="inlineStr"/>
       <c r="H206" t="n">
-        <v>1.059</v>
+        <v>1</v>
       </c>
       <c r="I206" t="n">
-        <v>0.9409999999999999</v>
+        <v>1</v>
       </c>
       <c r="J206" t="n">
         <v>0.85</v>
@@ -27464,10 +27464,10 @@
       <c r="F207" t="inlineStr"/>
       <c r="G207" t="inlineStr"/>
       <c r="H207" t="n">
-        <v>1.059</v>
+        <v>1</v>
       </c>
       <c r="I207" t="n">
-        <v>0.9409999999999999</v>
+        <v>1</v>
       </c>
       <c r="J207" t="n">
         <v>0.85</v>
@@ -27595,10 +27595,10 @@
       <c r="F208" t="inlineStr"/>
       <c r="G208" t="inlineStr"/>
       <c r="H208" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I208" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J208" t="n">
         <v>0.625</v>
@@ -27726,10 +27726,10 @@
       <c r="F209" t="inlineStr"/>
       <c r="G209" t="inlineStr"/>
       <c r="H209" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I209" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J209" t="n">
         <v>0</v>
@@ -27857,10 +27857,10 @@
       <c r="F210" t="inlineStr"/>
       <c r="G210" t="inlineStr"/>
       <c r="H210" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I210" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J210" t="n">
         <v>0</v>
@@ -28512,10 +28512,10 @@
       <c r="F215" t="inlineStr"/>
       <c r="G215" t="inlineStr"/>
       <c r="H215" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I215" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J215" t="n">
         <v>0.03</v>
@@ -28643,10 +28643,10 @@
       <c r="F216" t="inlineStr"/>
       <c r="G216" t="inlineStr"/>
       <c r="H216" t="n">
-        <v>1.667</v>
+        <v>1</v>
       </c>
       <c r="I216" t="n">
-        <v>0.333</v>
+        <v>1</v>
       </c>
       <c r="J216" t="n">
         <v>0.6</v>
@@ -28774,10 +28774,10 @@
       <c r="F217" t="inlineStr"/>
       <c r="G217" t="inlineStr"/>
       <c r="H217" t="n">
-        <v>2.86</v>
+        <v>1</v>
       </c>
       <c r="I217" t="n">
-        <v>0.14</v>
+        <v>1</v>
       </c>
       <c r="J217" t="n">
         <v>0.6</v>
@@ -28905,10 +28905,10 @@
       <c r="F218" t="inlineStr"/>
       <c r="G218" t="inlineStr"/>
       <c r="H218" t="n">
-        <v>2.86</v>
+        <v>1</v>
       </c>
       <c r="I218" t="n">
-        <v>0.14</v>
+        <v>1</v>
       </c>
       <c r="J218" t="n">
         <v>0.1</v>
@@ -29036,10 +29036,10 @@
       <c r="F219" t="inlineStr"/>
       <c r="G219" t="inlineStr"/>
       <c r="H219" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I219" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J219" t="n">
         <v>0.03</v>
@@ -29167,10 +29167,10 @@
       <c r="F220" t="inlineStr"/>
       <c r="G220" t="inlineStr"/>
       <c r="H220" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I220" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J220" t="n">
         <v>0.03</v>
@@ -29298,10 +29298,10 @@
       <c r="F221" t="inlineStr"/>
       <c r="G221" t="inlineStr"/>
       <c r="H221" t="n">
-        <v>1.667</v>
+        <v>1</v>
       </c>
       <c r="I221" t="n">
-        <v>0.333</v>
+        <v>1</v>
       </c>
       <c r="J221" t="n">
         <v>0.6</v>
@@ -29429,10 +29429,10 @@
       <c r="F222" t="inlineStr"/>
       <c r="G222" t="inlineStr"/>
       <c r="H222" t="n">
-        <v>1.44</v>
+        <v>1</v>
       </c>
       <c r="I222" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J222" t="n">
         <v>0.5</v>
@@ -29560,10 +29560,10 @@
       <c r="F223" t="inlineStr"/>
       <c r="G223" t="inlineStr"/>
       <c r="H223" t="n">
-        <v>2.67</v>
+        <v>1</v>
       </c>
       <c r="I223" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J223" t="n">
         <v>0.3</v>
@@ -29691,10 +29691,10 @@
       <c r="F224" t="inlineStr"/>
       <c r="G224" t="inlineStr"/>
       <c r="H224" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I224" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J224" t="n">
         <v>0.25</v>
@@ -29822,10 +29822,10 @@
       <c r="F225" t="inlineStr"/>
       <c r="G225" t="inlineStr"/>
       <c r="H225" t="n">
-        <v>1.39</v>
+        <v>1</v>
       </c>
       <c r="I225" t="n">
-        <v>0.46</v>
+        <v>1</v>
       </c>
       <c r="J225" t="n">
         <v>0.865</v>
@@ -29953,10 +29953,10 @@
       <c r="F226" t="inlineStr"/>
       <c r="G226" t="inlineStr"/>
       <c r="H226" t="n">
-        <v>1.39</v>
+        <v>1</v>
       </c>
       <c r="I226" t="n">
-        <v>0.46</v>
+        <v>1</v>
       </c>
       <c r="J226" t="n">
         <v>0.865</v>

</xml_diff>

<commit_message>
committing for state lock--used to run sisepuede_run_2023-10-06T20:10:09.932282
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_ce_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_ce_calibrated.xlsx
@@ -451,22 +451,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -1128,7 +1128,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_advanced_aerobic</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>53</v>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -1259,7 +1261,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>53</v>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -1390,7 +1394,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_latrine_improved</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>53</v>
+      </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -1521,7 +1527,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_latrine_unimproved</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>53</v>
+      </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -1652,7 +1660,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_primary</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>53</v>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -1783,7 +1793,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>53</v>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -1914,7 +1926,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>53</v>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -2045,7 +2059,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_septic</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>53</v>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
@@ -2176,7 +2192,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>53</v>
+      </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
@@ -2307,7 +2325,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>53</v>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -2438,7 +2458,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_advanced_aerobic</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>54</v>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
@@ -2569,7 +2591,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>54</v>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
@@ -2700,7 +2724,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_latrine_improved</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>54</v>
+      </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -2831,7 +2857,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_latrine_unimproved</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>54</v>
+      </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
@@ -2962,7 +2990,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_primary</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>54</v>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
@@ -3093,7 +3123,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="n">
+        <v>54</v>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
@@ -3224,7 +3256,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="n">
+        <v>54</v>
+      </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
@@ -3355,7 +3389,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_septic</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>54</v>
+      </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
@@ -3486,7 +3522,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>54</v>
+      </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
@@ -3617,7 +3655,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>54</v>
+      </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
@@ -3748,7 +3788,9 @@
           <t>frac_wali_ww_industrial_treatment_path_advanced_aerobic</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>55</v>
+      </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
@@ -3879,7 +3921,9 @@
           <t>frac_wali_ww_industrial_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="n">
+        <v>55</v>
+      </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
@@ -4010,7 +4054,9 @@
           <t>frac_wali_ww_industrial_treatment_path_latrine_improved</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>55</v>
+      </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -4141,7 +4187,9 @@
           <t>frac_wali_ww_industrial_treatment_path_latrine_unimproved</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="n">
+        <v>55</v>
+      </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
@@ -4272,7 +4320,9 @@
           <t>frac_wali_ww_industrial_treatment_path_primary</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="n">
+        <v>55</v>
+      </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
@@ -4403,7 +4453,9 @@
           <t>frac_wali_ww_industrial_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="n">
+        <v>55</v>
+      </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
@@ -4534,7 +4586,9 @@
           <t>frac_wali_ww_industrial_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="n">
+        <v>55</v>
+      </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
@@ -4665,7 +4719,9 @@
           <t>frac_wali_ww_industrial_treatment_path_septic</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
+      <c r="C33" t="n">
+        <v>55</v>
+      </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
@@ -4796,7 +4852,9 @@
           <t>frac_wali_ww_industrial_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="n">
+        <v>55</v>
+      </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
@@ -4927,7 +4985,9 @@
           <t>frac_wali_ww_industrial_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
+      <c r="C35" t="n">
+        <v>55</v>
+      </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
@@ -14359,7 +14419,9 @@
           <t>frac_waso_initial_composition_ind_chemical_industrial</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr"/>
+      <c r="C107" t="n">
+        <v>56</v>
+      </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="inlineStr"/>
@@ -14490,7 +14552,9 @@
           <t>frac_waso_initial_composition_ind_food</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr"/>
+      <c r="C108" t="n">
+        <v>56</v>
+      </c>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr"/>
@@ -14621,7 +14685,9 @@
           <t>frac_waso_initial_composition_ind_glass</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr"/>
+      <c r="C109" t="n">
+        <v>56</v>
+      </c>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr"/>
@@ -14752,7 +14818,9 @@
           <t>frac_waso_initial_composition_ind_metal</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr"/>
+      <c r="C110" t="n">
+        <v>56</v>
+      </c>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="inlineStr"/>
@@ -14883,7 +14951,9 @@
           <t>frac_waso_initial_composition_ind_nappies</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr"/>
+      <c r="C111" t="n">
+        <v>56</v>
+      </c>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="inlineStr"/>
@@ -15014,7 +15084,9 @@
           <t>frac_waso_initial_composition_ind_other</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr"/>
+      <c r="C112" t="n">
+        <v>56</v>
+      </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr"/>
@@ -15145,7 +15217,9 @@
           <t>frac_waso_initial_composition_ind_paper</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr"/>
+      <c r="C113" t="n">
+        <v>56</v>
+      </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="inlineStr"/>
@@ -15276,7 +15350,9 @@
           <t>frac_waso_initial_composition_ind_plastic</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr"/>
+      <c r="C114" t="n">
+        <v>56</v>
+      </c>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="inlineStr"/>
@@ -15407,7 +15483,9 @@
           <t>frac_waso_initial_composition_ind_rubber_leather</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr"/>
+      <c r="C115" t="n">
+        <v>56</v>
+      </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr"/>
@@ -15538,7 +15616,9 @@
           <t>frac_waso_initial_composition_ind_sludge</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr"/>
+      <c r="C116" t="n">
+        <v>56</v>
+      </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr"/>
@@ -15669,7 +15749,9 @@
           <t>frac_waso_initial_composition_ind_textiles</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr"/>
+      <c r="C117" t="n">
+        <v>56</v>
+      </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr"/>
@@ -15800,7 +15882,9 @@
           <t>frac_waso_initial_composition_ind_wood</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr"/>
+      <c r="C118" t="n">
+        <v>56</v>
+      </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr"/>
@@ -15931,7 +16015,9 @@
           <t>frac_waso_initial_composition_ind_yard</t>
         </is>
       </c>
-      <c r="C119" t="inlineStr"/>
+      <c r="C119" t="n">
+        <v>56</v>
+      </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr"/>
@@ -16062,7 +16148,9 @@
           <t>frac_waso_initial_composition_mun_chemical_industrial</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr"/>
+      <c r="C120" t="n">
+        <v>57</v>
+      </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr"/>
@@ -16193,7 +16281,9 @@
           <t>frac_waso_initial_composition_mun_food</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr"/>
+      <c r="C121" t="n">
+        <v>57</v>
+      </c>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
       <c r="F121" t="inlineStr"/>
@@ -16324,7 +16414,9 @@
           <t>frac_waso_initial_composition_mun_glass</t>
         </is>
       </c>
-      <c r="C122" t="inlineStr"/>
+      <c r="C122" t="n">
+        <v>57</v>
+      </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr"/>
@@ -16455,7 +16547,9 @@
           <t>frac_waso_initial_composition_mun_metal</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr"/>
+      <c r="C123" t="n">
+        <v>57</v>
+      </c>
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr"/>
@@ -16586,7 +16680,9 @@
           <t>frac_waso_initial_composition_mun_nappies</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr"/>
+      <c r="C124" t="n">
+        <v>57</v>
+      </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
       <c r="F124" t="inlineStr"/>
@@ -16717,7 +16813,9 @@
           <t>frac_waso_initial_composition_mun_other</t>
         </is>
       </c>
-      <c r="C125" t="inlineStr"/>
+      <c r="C125" t="n">
+        <v>57</v>
+      </c>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
       <c r="F125" t="inlineStr"/>
@@ -16848,7 +16946,9 @@
           <t>frac_waso_initial_composition_mun_paper</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr"/>
+      <c r="C126" t="n">
+        <v>57</v>
+      </c>
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
@@ -16979,7 +17079,9 @@
           <t>frac_waso_initial_composition_mun_plastic</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr"/>
+      <c r="C127" t="n">
+        <v>57</v>
+      </c>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
@@ -17110,7 +17212,9 @@
           <t>frac_waso_initial_composition_mun_rubber_leather</t>
         </is>
       </c>
-      <c r="C128" t="inlineStr"/>
+      <c r="C128" t="n">
+        <v>57</v>
+      </c>
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="inlineStr"/>
@@ -17241,7 +17345,9 @@
           <t>frac_waso_initial_composition_mun_sludge</t>
         </is>
       </c>
-      <c r="C129" t="inlineStr"/>
+      <c r="C129" t="n">
+        <v>57</v>
+      </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="inlineStr"/>
@@ -17372,7 +17478,9 @@
           <t>frac_waso_initial_composition_mun_textiles</t>
         </is>
       </c>
-      <c r="C130" t="inlineStr"/>
+      <c r="C130" t="n">
+        <v>57</v>
+      </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="inlineStr"/>
@@ -17503,7 +17611,9 @@
           <t>frac_waso_initial_composition_mun_wood</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr"/>
+      <c r="C131" t="n">
+        <v>57</v>
+      </c>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
@@ -17634,7 +17744,9 @@
           <t>frac_waso_initial_composition_mun_yard</t>
         </is>
       </c>
-      <c r="C132" t="inlineStr"/>
+      <c r="C132" t="n">
+        <v>57</v>
+      </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="inlineStr"/>
@@ -18289,7 +18401,9 @@
           <t>frac_waso_non_recycled_incinerated</t>
         </is>
       </c>
-      <c r="C137" t="inlineStr"/>
+      <c r="C137" t="n">
+        <v>58</v>
+      </c>
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr"/>
       <c r="F137" t="inlineStr"/>
@@ -18420,7 +18534,9 @@
           <t>frac_waso_non_recycled_landfilled</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr"/>
+      <c r="C138" t="n">
+        <v>58</v>
+      </c>
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="inlineStr"/>
@@ -18551,7 +18667,9 @@
           <t>frac_waso_non_recycled_open_dump</t>
         </is>
       </c>
-      <c r="C139" t="inlineStr"/>
+      <c r="C139" t="n">
+        <v>58</v>
+      </c>
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="inlineStr"/>
       <c r="F139" t="inlineStr"/>
@@ -30100,22 +30218,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -30253,7 +30371,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_septic</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>53</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -30384,7 +30504,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>53</v>
+      </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
@@ -30515,7 +30637,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>53</v>
+      </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -30646,7 +30770,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_advanced_aerobic</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>54</v>
+      </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -30777,7 +30903,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>54</v>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -30908,7 +31036,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>54</v>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -31039,7 +31169,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>54</v>
+      </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -31170,7 +31302,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>54</v>
+      </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -31301,7 +31435,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>54</v>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -31432,7 +31568,9 @@
           <t>frac_wali_ww_industrial_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>55</v>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -31563,7 +31701,9 @@
           <t>frac_wali_ww_industrial_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>55</v>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -31694,7 +31834,9 @@
           <t>frac_wali_ww_industrial_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>55</v>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
@@ -31825,7 +31967,9 @@
           <t>frac_wali_ww_industrial_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>55</v>
+      </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
@@ -31956,7 +32100,9 @@
           <t>frac_wali_ww_industrial_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>55</v>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -32087,7 +32233,9 @@
           <t>frac_waso_non_recycled_landfilled</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>58</v>
+      </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
@@ -32218,7 +32366,9 @@
           <t>frac_waso_non_recycled_open_dump</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>58</v>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
@@ -33287,22 +33437,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -34378,22 +34528,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -35600,22 +35750,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -35753,7 +35903,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_septic</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>53</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -35884,7 +36036,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>53</v>
+      </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
@@ -36015,7 +36169,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>53</v>
+      </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -36146,7 +36302,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_advanced_aerobic</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>54</v>
+      </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -36277,7 +36435,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>54</v>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -36408,7 +36568,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>54</v>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -36539,7 +36701,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>54</v>
+      </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -36670,7 +36834,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>54</v>
+      </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -36801,7 +36967,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>54</v>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -36932,7 +37100,9 @@
           <t>frac_wali_ww_industrial_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>55</v>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -37063,7 +37233,9 @@
           <t>frac_wali_ww_industrial_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>55</v>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -37194,7 +37366,9 @@
           <t>frac_wali_ww_industrial_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>55</v>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
@@ -37325,7 +37499,9 @@
           <t>frac_wali_ww_industrial_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>55</v>
+      </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
@@ -37456,7 +37632,9 @@
           <t>frac_wali_ww_industrial_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>55</v>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -39028,7 +39206,9 @@
           <t>frac_waso_non_recycled_landfilled</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="n">
+        <v>58</v>
+      </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
@@ -39159,7 +39339,9 @@
           <t>frac_waso_non_recycled_open_dump</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>58</v>
+      </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -40752,22 +40934,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>normalize_group</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>trajgroup_no_vary_q</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -40905,7 +41087,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_septic</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>53</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -41036,7 +41220,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>53</v>
+      </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
@@ -41167,7 +41353,9 @@
           <t>frac_wali_ww_domestic_rural_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>53</v>
+      </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -41298,7 +41486,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_advanced_aerobic</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>54</v>
+      </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -41429,7 +41619,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>54</v>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -41560,7 +41752,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>54</v>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -41691,7 +41885,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>54</v>
+      </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -41822,7 +42018,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>54</v>
+      </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -41953,7 +42151,9 @@
           <t>frac_wali_ww_domestic_urban_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>54</v>
+      </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -42084,7 +42284,9 @@
           <t>frac_wali_ww_industrial_treatment_path_advanced_anaerobic</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>55</v>
+      </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -42215,7 +42417,9 @@
           <t>frac_wali_ww_industrial_treatment_path_secondary_aerobic</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>55</v>
+      </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -42346,7 +42550,9 @@
           <t>frac_wali_ww_industrial_treatment_path_secondary_anaerobic</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>55</v>
+      </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
@@ -42477,7 +42683,9 @@
           <t>frac_wali_ww_industrial_treatment_path_untreated_no_sewerage</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>55</v>
+      </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
@@ -42608,7 +42816,9 @@
           <t>frac_wali_ww_industrial_treatment_path_untreated_with_sewerage</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>55</v>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -44180,7 +44390,9 @@
           <t>frac_waso_non_recycled_landfilled</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="n">
+        <v>58</v>
+      </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
@@ -44311,7 +44523,9 @@
           <t>frac_waso_non_recycled_open_dump</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>58</v>
+      </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>

</xml_diff>

<commit_message>
Updated templates to include key strategies and re-pushed. Includes some minor updates to transformation scripts
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_ce_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_ce_calibrated.xlsx
@@ -14434,7 +14434,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
@@ -14567,7 +14567,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
@@ -14700,7 +14700,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
@@ -14833,7 +14833,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
@@ -14966,7 +14966,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
@@ -15099,7 +15099,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
@@ -15232,7 +15232,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
@@ -15365,7 +15365,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
@@ -15498,7 +15498,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
@@ -15631,7 +15631,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
@@ -15764,7 +15764,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
@@ -15897,7 +15897,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
@@ -16030,7 +16030,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
@@ -16163,7 +16163,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
@@ -16296,7 +16296,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
@@ -16429,7 +16429,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
@@ -16562,7 +16562,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
@@ -16695,7 +16695,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
@@ -16828,7 +16828,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
@@ -16961,7 +16961,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
@@ -17094,7 +17094,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
@@ -17227,7 +17227,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
@@ -17360,7 +17360,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
@@ -17493,7 +17493,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
@@ -17626,7 +17626,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
@@ -17759,7 +17759,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>

</xml_diff>